<commit_message>
add ovs & modify virtual plan
</commit_message>
<xml_diff>
--- a/list/virtualization.xlsx
+++ b/list/virtualization.xlsx
@@ -11,14 +11,14 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$155</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$173</definedName>
   </definedNames>
   <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214">
   <si>
     <t>测试项目</t>
   </si>
@@ -2592,6 +2592,66 @@
   </si>
   <si>
     <t>kops.md</t>
+  </si>
+  <si>
+    <t>Open VSwitch</t>
+  </si>
+  <si>
+    <t>安装工具包</t>
+  </si>
+  <si>
+    <t>ovs.sh</t>
+  </si>
+  <si>
+    <t>安装open vswitch</t>
+  </si>
+  <si>
+    <t>启动open vswitch服务</t>
+  </si>
+  <si>
+    <t>启动ovsdb-server数据库</t>
+  </si>
+  <si>
+    <t>初始化ovs数据库</t>
+  </si>
+  <si>
+    <t>开启ovs-vswitchd后台进程</t>
+  </si>
+  <si>
+    <t>查看open vswitch版本</t>
+  </si>
+  <si>
+    <t>增加ovs虚拟网桥br0</t>
+  </si>
+  <si>
+    <t>列举所有ovs网桥</t>
+  </si>
+  <si>
+    <t>启用虚拟网桥br0</t>
+  </si>
+  <si>
+    <t>将物理网卡挂接到网桥</t>
+  </si>
+  <si>
+    <t>列出网桥中所有端口</t>
+  </si>
+  <si>
+    <t>列出所有挂接到网卡的网桥</t>
+  </si>
+  <si>
+    <t>查看open vswitch的网络状态</t>
+  </si>
+  <si>
+    <t>删除网桥上已挂接的网口</t>
+  </si>
+  <si>
+    <t>删除网桥</t>
+  </si>
+  <si>
+    <t>停止open vswitch服务</t>
+  </si>
+  <si>
+    <t>卸载open vswitch安装包</t>
   </si>
   <si>
     <t>cadvisor
@@ -2682,10 +2742,10 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="m&quot;／&quot;d&quot;／&quot;yyyy"/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="176" formatCode="m&quot;／&quot;d&quot;／&quot;yyyy"/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="40">
     <font>
@@ -2827,9 +2887,46 @@
       <charset val="134"/>
     </font>
     <font>
-      <u/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2842,62 +2939,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2919,9 +2963,39 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2939,23 +3013,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3000,7 +3060,145 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3012,139 +3210,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3157,24 +3235,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3317,6 +3377,19 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right style="thin">
         <color auto="1"/>
@@ -3327,19 +3400,6 @@
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -3466,15 +3526,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -3483,141 +3534,150 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="21" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="34" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="35" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="38" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="9" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="9" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="21" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="13" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="10" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="11" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="14" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="9" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyBorder="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyBorder="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="21" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3626,7 +3686,7 @@
     </xf>
     <xf numFmtId="9" fontId="21" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top"/>
     </xf>
@@ -3752,13 +3812,22 @@
     <xf numFmtId="0" fontId="16" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="10" xfId="44" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="11" xfId="44" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="10" xfId="44" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4205,12 +4274,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:I157"/>
+  <dimension ref="A1:I175"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A133" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A139" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="D125" sqref="D125:D135"/>
+      <selection pane="bottomLeft" activeCell="D153" sqref="D153:D170"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
@@ -7379,16 +7448,16 @@
       <c r="D136" s="38" t="s">
         <v>168</v>
       </c>
-      <c r="E136" s="50" t="s">
+      <c r="E136" s="53" t="s">
         <v>169</v>
       </c>
-      <c r="F136" s="51" t="s">
+      <c r="F136" s="54" t="s">
         <v>62</v>
       </c>
-      <c r="G136" s="52" t="s">
-        <v>15</v>
-      </c>
-      <c r="H136" s="53" t="s">
+      <c r="G136" s="55" t="s">
+        <v>15</v>
+      </c>
+      <c r="H136" s="56" t="s">
         <v>13</v>
       </c>
       <c r="I136" s="33"/>
@@ -7402,16 +7471,16 @@
         <v>167</v>
       </c>
       <c r="D137" s="38"/>
-      <c r="E137" s="50" t="s">
+      <c r="E137" s="53" t="s">
         <v>169</v>
       </c>
-      <c r="F137" s="51" t="s">
+      <c r="F137" s="54" t="s">
         <v>62</v>
       </c>
-      <c r="G137" s="52" t="s">
-        <v>15</v>
-      </c>
-      <c r="H137" s="53" t="s">
+      <c r="G137" s="55" t="s">
+        <v>15</v>
+      </c>
+      <c r="H137" s="56" t="s">
         <v>13</v>
       </c>
       <c r="I137" s="33"/>
@@ -7425,16 +7494,16 @@
         <v>167</v>
       </c>
       <c r="D138" s="38"/>
-      <c r="E138" s="50" t="s">
+      <c r="E138" s="53" t="s">
         <v>169</v>
       </c>
-      <c r="F138" s="51" t="s">
+      <c r="F138" s="54" t="s">
         <v>62</v>
       </c>
-      <c r="G138" s="52" t="s">
-        <v>15</v>
-      </c>
-      <c r="H138" s="53" t="s">
+      <c r="G138" s="55" t="s">
+        <v>15</v>
+      </c>
+      <c r="H138" s="56" t="s">
         <v>13</v>
       </c>
       <c r="I138" s="33"/>
@@ -7448,16 +7517,16 @@
         <v>167</v>
       </c>
       <c r="D139" s="38"/>
-      <c r="E139" s="50" t="s">
+      <c r="E139" s="53" t="s">
         <v>169</v>
       </c>
-      <c r="F139" s="51" t="s">
+      <c r="F139" s="54" t="s">
         <v>62</v>
       </c>
-      <c r="G139" s="52" t="s">
-        <v>15</v>
-      </c>
-      <c r="H139" s="53" t="s">
+      <c r="G139" s="55" t="s">
+        <v>15</v>
+      </c>
+      <c r="H139" s="56" t="s">
         <v>13</v>
       </c>
       <c r="I139" s="33"/>
@@ -7471,16 +7540,16 @@
         <v>167</v>
       </c>
       <c r="D140" s="38"/>
-      <c r="E140" s="50" t="s">
+      <c r="E140" s="53" t="s">
         <v>169</v>
       </c>
-      <c r="F140" s="51" t="s">
+      <c r="F140" s="54" t="s">
         <v>62</v>
       </c>
-      <c r="G140" s="52" t="s">
-        <v>15</v>
-      </c>
-      <c r="H140" s="53" t="s">
+      <c r="G140" s="55" t="s">
+        <v>15</v>
+      </c>
+      <c r="H140" s="56" t="s">
         <v>13</v>
       </c>
       <c r="I140" s="33"/>
@@ -7494,16 +7563,16 @@
         <v>167</v>
       </c>
       <c r="D141" s="38"/>
-      <c r="E141" s="50" t="s">
+      <c r="E141" s="53" t="s">
         <v>169</v>
       </c>
-      <c r="F141" s="51" t="s">
+      <c r="F141" s="54" t="s">
         <v>62</v>
       </c>
-      <c r="G141" s="52" t="s">
-        <v>15</v>
-      </c>
-      <c r="H141" s="53" t="s">
+      <c r="G141" s="55" t="s">
+        <v>15</v>
+      </c>
+      <c r="H141" s="56" t="s">
         <v>13</v>
       </c>
       <c r="I141" s="33"/>
@@ -7517,16 +7586,16 @@
         <v>167</v>
       </c>
       <c r="D142" s="38"/>
-      <c r="E142" s="50" t="s">
+      <c r="E142" s="53" t="s">
         <v>169</v>
       </c>
-      <c r="F142" s="51" t="s">
+      <c r="F142" s="54" t="s">
         <v>62</v>
       </c>
-      <c r="G142" s="52" t="s">
-        <v>15</v>
-      </c>
-      <c r="H142" s="53" t="s">
+      <c r="G142" s="55" t="s">
+        <v>15</v>
+      </c>
+      <c r="H142" s="56" t="s">
         <v>13</v>
       </c>
       <c r="I142" s="33"/>
@@ -7540,16 +7609,16 @@
         <v>167</v>
       </c>
       <c r="D143" s="38"/>
-      <c r="E143" s="50" t="s">
+      <c r="E143" s="53" t="s">
         <v>169</v>
       </c>
-      <c r="F143" s="51" t="s">
+      <c r="F143" s="54" t="s">
         <v>62</v>
       </c>
-      <c r="G143" s="52" t="s">
-        <v>15</v>
-      </c>
-      <c r="H143" s="53" t="s">
+      <c r="G143" s="55" t="s">
+        <v>15</v>
+      </c>
+      <c r="H143" s="56" t="s">
         <v>13</v>
       </c>
       <c r="I143" s="33"/>
@@ -7563,16 +7632,16 @@
         <v>167</v>
       </c>
       <c r="D144" s="38"/>
-      <c r="E144" s="50" t="s">
+      <c r="E144" s="53" t="s">
         <v>169</v>
       </c>
-      <c r="F144" s="51" t="s">
+      <c r="F144" s="54" t="s">
         <v>62</v>
       </c>
-      <c r="G144" s="52" t="s">
-        <v>15</v>
-      </c>
-      <c r="H144" s="53" t="s">
+      <c r="G144" s="55" t="s">
+        <v>15</v>
+      </c>
+      <c r="H144" s="56" t="s">
         <v>13</v>
       </c>
       <c r="I144" s="33"/>
@@ -7586,16 +7655,16 @@
         <v>167</v>
       </c>
       <c r="D145" s="38"/>
-      <c r="E145" s="50" t="s">
+      <c r="E145" s="53" t="s">
         <v>169</v>
       </c>
-      <c r="F145" s="51" t="s">
+      <c r="F145" s="54" t="s">
         <v>62</v>
       </c>
-      <c r="G145" s="52" t="s">
-        <v>15</v>
-      </c>
-      <c r="H145" s="53" t="s">
+      <c r="G145" s="55" t="s">
+        <v>15</v>
+      </c>
+      <c r="H145" s="56" t="s">
         <v>13</v>
       </c>
       <c r="I145" s="33"/>
@@ -7609,16 +7678,16 @@
         <v>167</v>
       </c>
       <c r="D146" s="38"/>
-      <c r="E146" s="50" t="s">
+      <c r="E146" s="53" t="s">
         <v>169</v>
       </c>
-      <c r="F146" s="51" t="s">
+      <c r="F146" s="54" t="s">
         <v>62</v>
       </c>
-      <c r="G146" s="52" t="s">
-        <v>15</v>
-      </c>
-      <c r="H146" s="53" t="s">
+      <c r="G146" s="55" t="s">
+        <v>15</v>
+      </c>
+      <c r="H146" s="56" t="s">
         <v>13</v>
       </c>
       <c r="I146" s="33"/>
@@ -7632,16 +7701,16 @@
         <v>167</v>
       </c>
       <c r="D147" s="38"/>
-      <c r="E147" s="50" t="s">
+      <c r="E147" s="53" t="s">
         <v>169</v>
       </c>
-      <c r="F147" s="51" t="s">
+      <c r="F147" s="54" t="s">
         <v>62</v>
       </c>
-      <c r="G147" s="52" t="s">
-        <v>15</v>
-      </c>
-      <c r="H147" s="53" t="s">
+      <c r="G147" s="55" t="s">
+        <v>15</v>
+      </c>
+      <c r="H147" s="56" t="s">
         <v>13</v>
       </c>
       <c r="I147" s="33"/>
@@ -7655,16 +7724,16 @@
         <v>167</v>
       </c>
       <c r="D148" s="38"/>
-      <c r="E148" s="50" t="s">
+      <c r="E148" s="53" t="s">
         <v>169</v>
       </c>
-      <c r="F148" s="51" t="s">
+      <c r="F148" s="54" t="s">
         <v>62</v>
       </c>
-      <c r="G148" s="52" t="s">
-        <v>15</v>
-      </c>
-      <c r="H148" s="53" t="s">
+      <c r="G148" s="55" t="s">
+        <v>15</v>
+      </c>
+      <c r="H148" s="56" t="s">
         <v>13</v>
       </c>
       <c r="I148" s="33"/>
@@ -7678,16 +7747,16 @@
         <v>167</v>
       </c>
       <c r="D149" s="38"/>
-      <c r="E149" s="50" t="s">
+      <c r="E149" s="53" t="s">
         <v>169</v>
       </c>
-      <c r="F149" s="51" t="s">
+      <c r="F149" s="54" t="s">
         <v>62</v>
       </c>
-      <c r="G149" s="52" t="s">
-        <v>15</v>
-      </c>
-      <c r="H149" s="53" t="s">
+      <c r="G149" s="55" t="s">
+        <v>15</v>
+      </c>
+      <c r="H149" s="56" t="s">
         <v>13</v>
       </c>
       <c r="I149" s="33"/>
@@ -7701,16 +7770,16 @@
         <v>167</v>
       </c>
       <c r="D150" s="38"/>
-      <c r="E150" s="50" t="s">
+      <c r="E150" s="53" t="s">
         <v>169</v>
       </c>
-      <c r="F150" s="51" t="s">
+      <c r="F150" s="54" t="s">
         <v>62</v>
       </c>
-      <c r="G150" s="52" t="s">
-        <v>15</v>
-      </c>
-      <c r="H150" s="53" t="s">
+      <c r="G150" s="55" t="s">
+        <v>15</v>
+      </c>
+      <c r="H150" s="56" t="s">
         <v>13</v>
       </c>
       <c r="I150" s="33"/>
@@ -7724,16 +7793,16 @@
         <v>167</v>
       </c>
       <c r="D151" s="38"/>
-      <c r="E151" s="50" t="s">
+      <c r="E151" s="53" t="s">
         <v>169</v>
       </c>
-      <c r="F151" s="51" t="s">
+      <c r="F151" s="54" t="s">
         <v>62</v>
       </c>
-      <c r="G151" s="52" t="s">
-        <v>15</v>
-      </c>
-      <c r="H151" s="53" t="s">
+      <c r="G151" s="55" t="s">
+        <v>15</v>
+      </c>
+      <c r="H151" s="56" t="s">
         <v>13</v>
       </c>
       <c r="I151" s="33"/>
@@ -7757,7 +7826,7 @@
       <c r="H152" s="18"/>
       <c r="I152" s="33"/>
     </row>
-    <row r="153" ht="13.5" customHeight="1" spans="1:9">
+    <row r="153" s="1" customFormat="1" ht="15" spans="1:9">
       <c r="A153" s="44" t="s">
         <v>187</v>
       </c>
@@ -7773,23 +7842,21 @@
       <c r="E153" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="F153" s="31" t="s">
-        <v>14</v>
-      </c>
-      <c r="G153" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="H153" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="I153" s="33" t="s">
+      <c r="F153" s="54" t="s">
+        <v>14</v>
+      </c>
+      <c r="G153" s="55" t="s">
+        <v>15</v>
+      </c>
+      <c r="H153" s="56" t="s">
+        <v>13</v>
+      </c>
+      <c r="I153" s="33"/>
+    </row>
+    <row r="154" s="1" customFormat="1" ht="15" spans="1:9">
+      <c r="A154" s="44"/>
+      <c r="B154" s="45" t="s">
         <v>190</v>
-      </c>
-    </row>
-    <row r="154" spans="1:9">
-      <c r="A154" s="47"/>
-      <c r="B154" s="45" t="s">
-        <v>191</v>
       </c>
       <c r="C154" s="25" t="s">
         <v>11</v>
@@ -7798,52 +7865,472 @@
       <c r="E154" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="F154" s="31" t="s">
-        <v>14</v>
-      </c>
-      <c r="G154" s="17" t="s">
+      <c r="F154" s="54" t="s">
+        <v>14</v>
+      </c>
+      <c r="G154" s="55" t="s">
+        <v>15</v>
+      </c>
+      <c r="H154" s="56" t="s">
+        <v>13</v>
+      </c>
+      <c r="I154" s="33"/>
+    </row>
+    <row r="155" s="1" customFormat="1" ht="15" spans="1:9">
+      <c r="A155" s="44"/>
+      <c r="B155" s="45" t="s">
+        <v>191</v>
+      </c>
+      <c r="C155" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="D155" s="46"/>
+      <c r="E155" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="F155" s="54" t="s">
+        <v>14</v>
+      </c>
+      <c r="G155" s="55" t="s">
+        <v>15</v>
+      </c>
+      <c r="H155" s="56" t="s">
+        <v>13</v>
+      </c>
+      <c r="I155" s="33"/>
+    </row>
+    <row r="156" s="1" customFormat="1" ht="15" spans="1:9">
+      <c r="A156" s="44"/>
+      <c r="B156" s="45" t="s">
+        <v>192</v>
+      </c>
+      <c r="C156" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="D156" s="46"/>
+      <c r="E156" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="F156" s="54" t="s">
+        <v>14</v>
+      </c>
+      <c r="G156" s="55" t="s">
+        <v>15</v>
+      </c>
+      <c r="H156" s="56" t="s">
+        <v>13</v>
+      </c>
+      <c r="I156" s="33"/>
+    </row>
+    <row r="157" s="1" customFormat="1" ht="15" spans="1:9">
+      <c r="A157" s="44"/>
+      <c r="B157" s="45" t="s">
+        <v>193</v>
+      </c>
+      <c r="C157" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="D157" s="46"/>
+      <c r="E157" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="F157" s="54" t="s">
+        <v>14</v>
+      </c>
+      <c r="G157" s="55" t="s">
+        <v>15</v>
+      </c>
+      <c r="H157" s="56" t="s">
+        <v>13</v>
+      </c>
+      <c r="I157" s="33"/>
+    </row>
+    <row r="158" s="1" customFormat="1" ht="15" spans="1:9">
+      <c r="A158" s="44"/>
+      <c r="B158" s="45" t="s">
+        <v>194</v>
+      </c>
+      <c r="C158" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="D158" s="46"/>
+      <c r="E158" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="F158" s="54" t="s">
+        <v>14</v>
+      </c>
+      <c r="G158" s="55" t="s">
+        <v>15</v>
+      </c>
+      <c r="H158" s="56" t="s">
+        <v>13</v>
+      </c>
+      <c r="I158" s="33"/>
+    </row>
+    <row r="159" s="1" customFormat="1" ht="15" spans="1:9">
+      <c r="A159" s="44"/>
+      <c r="B159" s="45" t="s">
+        <v>195</v>
+      </c>
+      <c r="C159" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="D159" s="46"/>
+      <c r="E159" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="F159" s="54" t="s">
+        <v>14</v>
+      </c>
+      <c r="G159" s="55" t="s">
+        <v>15</v>
+      </c>
+      <c r="H159" s="56" t="s">
+        <v>13</v>
+      </c>
+      <c r="I159" s="33"/>
+    </row>
+    <row r="160" s="1" customFormat="1" ht="15" spans="1:9">
+      <c r="A160" s="44"/>
+      <c r="B160" s="45" t="s">
+        <v>196</v>
+      </c>
+      <c r="C160" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="D160" s="46"/>
+      <c r="E160" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="F160" s="54" t="s">
+        <v>14</v>
+      </c>
+      <c r="G160" s="55" t="s">
+        <v>15</v>
+      </c>
+      <c r="H160" s="56" t="s">
+        <v>13</v>
+      </c>
+      <c r="I160" s="33"/>
+    </row>
+    <row r="161" s="1" customFormat="1" ht="15" spans="1:9">
+      <c r="A161" s="44"/>
+      <c r="B161" s="45" t="s">
+        <v>197</v>
+      </c>
+      <c r="C161" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="D161" s="46"/>
+      <c r="E161" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="F161" s="54" t="s">
+        <v>14</v>
+      </c>
+      <c r="G161" s="55" t="s">
+        <v>15</v>
+      </c>
+      <c r="H161" s="56" t="s">
+        <v>13</v>
+      </c>
+      <c r="I161" s="33"/>
+    </row>
+    <row r="162" s="1" customFormat="1" ht="15" spans="1:9">
+      <c r="A162" s="44"/>
+      <c r="B162" s="45" t="s">
+        <v>198</v>
+      </c>
+      <c r="C162" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="D162" s="46"/>
+      <c r="E162" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="F162" s="54" t="s">
+        <v>14</v>
+      </c>
+      <c r="G162" s="55" t="s">
+        <v>15</v>
+      </c>
+      <c r="H162" s="56" t="s">
+        <v>13</v>
+      </c>
+      <c r="I162" s="33"/>
+    </row>
+    <row r="163" s="1" customFormat="1" ht="15" spans="1:9">
+      <c r="A163" s="44"/>
+      <c r="B163" s="45" t="s">
+        <v>199</v>
+      </c>
+      <c r="C163" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="D163" s="46"/>
+      <c r="E163" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="F163" s="54" t="s">
+        <v>14</v>
+      </c>
+      <c r="G163" s="55" t="s">
+        <v>15</v>
+      </c>
+      <c r="H163" s="56" t="s">
+        <v>13</v>
+      </c>
+      <c r="I163" s="33"/>
+    </row>
+    <row r="164" s="1" customFormat="1" ht="15" spans="1:9">
+      <c r="A164" s="44"/>
+      <c r="B164" s="45" t="s">
+        <v>200</v>
+      </c>
+      <c r="C164" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="D164" s="46"/>
+      <c r="E164" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="F164" s="54" t="s">
+        <v>14</v>
+      </c>
+      <c r="G164" s="55" t="s">
+        <v>15</v>
+      </c>
+      <c r="H164" s="56" t="s">
+        <v>13</v>
+      </c>
+      <c r="I164" s="33"/>
+    </row>
+    <row r="165" s="1" customFormat="1" ht="15" spans="1:9">
+      <c r="A165" s="44"/>
+      <c r="B165" s="45" t="s">
+        <v>201</v>
+      </c>
+      <c r="C165" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="D165" s="46"/>
+      <c r="E165" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="F165" s="54" t="s">
+        <v>14</v>
+      </c>
+      <c r="G165" s="55" t="s">
+        <v>15</v>
+      </c>
+      <c r="H165" s="56" t="s">
+        <v>13</v>
+      </c>
+      <c r="I165" s="33"/>
+    </row>
+    <row r="166" s="1" customFormat="1" ht="15" spans="1:9">
+      <c r="A166" s="44"/>
+      <c r="B166" s="45" t="s">
+        <v>202</v>
+      </c>
+      <c r="C166" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="D166" s="46"/>
+      <c r="E166" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="F166" s="54" t="s">
+        <v>14</v>
+      </c>
+      <c r="G166" s="55" t="s">
+        <v>15</v>
+      </c>
+      <c r="H166" s="56" t="s">
+        <v>13</v>
+      </c>
+      <c r="I166" s="33"/>
+    </row>
+    <row r="167" s="1" customFormat="1" ht="15" spans="1:9">
+      <c r="A167" s="44"/>
+      <c r="B167" s="45" t="s">
+        <v>203</v>
+      </c>
+      <c r="C167" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="D167" s="46"/>
+      <c r="E167" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="F167" s="54" t="s">
+        <v>14</v>
+      </c>
+      <c r="G167" s="55" t="s">
+        <v>15</v>
+      </c>
+      <c r="H167" s="56" t="s">
+        <v>13</v>
+      </c>
+      <c r="I167" s="33"/>
+    </row>
+    <row r="168" s="1" customFormat="1" ht="15" spans="1:9">
+      <c r="A168" s="44"/>
+      <c r="B168" s="45" t="s">
+        <v>204</v>
+      </c>
+      <c r="C168" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="D168" s="46"/>
+      <c r="E168" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="F168" s="54" t="s">
+        <v>14</v>
+      </c>
+      <c r="G168" s="55" t="s">
+        <v>15</v>
+      </c>
+      <c r="H168" s="56" t="s">
+        <v>13</v>
+      </c>
+      <c r="I168" s="33"/>
+    </row>
+    <row r="169" s="1" customFormat="1" ht="15" spans="1:9">
+      <c r="A169" s="44"/>
+      <c r="B169" s="45" t="s">
+        <v>205</v>
+      </c>
+      <c r="C169" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="D169" s="46"/>
+      <c r="E169" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="F169" s="54" t="s">
+        <v>14</v>
+      </c>
+      <c r="G169" s="55" t="s">
+        <v>15</v>
+      </c>
+      <c r="H169" s="56" t="s">
+        <v>13</v>
+      </c>
+      <c r="I169" s="33"/>
+    </row>
+    <row r="170" s="1" customFormat="1" ht="15" spans="1:9">
+      <c r="A170" s="44"/>
+      <c r="B170" s="45" t="s">
+        <v>206</v>
+      </c>
+      <c r="C170" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="D170" s="46"/>
+      <c r="E170" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="F170" s="54" t="s">
+        <v>14</v>
+      </c>
+      <c r="G170" s="55" t="s">
+        <v>15</v>
+      </c>
+      <c r="H170" s="56" t="s">
+        <v>13</v>
+      </c>
+      <c r="I170" s="33"/>
+    </row>
+    <row r="171" ht="13.5" customHeight="1" spans="1:9">
+      <c r="A171" s="47" t="s">
+        <v>207</v>
+      </c>
+      <c r="B171" s="48" t="s">
+        <v>208</v>
+      </c>
+      <c r="C171" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="D171" s="49" t="s">
+        <v>209</v>
+      </c>
+      <c r="E171" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="F171" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="G171" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="H171" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="I171" s="33" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="172" spans="1:9">
+      <c r="A172" s="50"/>
+      <c r="B172" s="48" t="s">
+        <v>211</v>
+      </c>
+      <c r="C172" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="D172" s="49"/>
+      <c r="E172" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="F172" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="G172" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="H154" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="I154" s="33" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="155" spans="1:9">
-      <c r="A155" s="47"/>
-      <c r="B155" s="48" t="s">
-        <v>192</v>
-      </c>
-      <c r="C155" s="49" t="s">
-        <v>11</v>
-      </c>
-      <c r="D155" s="46"/>
-      <c r="E155" s="54" t="s">
-        <v>13</v>
-      </c>
-      <c r="F155" s="55" t="s">
-        <v>14</v>
-      </c>
-      <c r="G155" s="17" t="s">
+      <c r="H172" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="I172" s="33" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="173" spans="1:9">
+      <c r="A173" s="50"/>
+      <c r="B173" s="51" t="s">
+        <v>212</v>
+      </c>
+      <c r="C173" s="52" t="s">
+        <v>11</v>
+      </c>
+      <c r="D173" s="49"/>
+      <c r="E173" s="57" t="s">
+        <v>13</v>
+      </c>
+      <c r="F173" s="58" t="s">
+        <v>14</v>
+      </c>
+      <c r="G173" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="H155" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="I155" s="56" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="157" spans="1:1">
-      <c r="A157" s="2" t="s">
-        <v>193</v>
+      <c r="H173" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="I173" s="59" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="175" spans="1:1">
+      <c r="A175" s="2" t="s">
+        <v>213</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I155"/>
-  <mergeCells count="18">
+  <autoFilter ref="A1:I173"/>
+  <mergeCells count="20">
     <mergeCell ref="A2:A14"/>
     <mergeCell ref="A15:A30"/>
     <mergeCell ref="A31:A41"/>
@@ -7852,7 +8339,8 @@
     <mergeCell ref="A107:A124"/>
     <mergeCell ref="A125:A135"/>
     <mergeCell ref="A136:A151"/>
-    <mergeCell ref="A153:A155"/>
+    <mergeCell ref="A153:A170"/>
+    <mergeCell ref="A171:A173"/>
     <mergeCell ref="D2:D14"/>
     <mergeCell ref="D15:D30"/>
     <mergeCell ref="D31:D41"/>
@@ -7861,9 +8349,10 @@
     <mergeCell ref="D107:D124"/>
     <mergeCell ref="D125:D135"/>
     <mergeCell ref="D136:D151"/>
-    <mergeCell ref="D153:D155"/>
+    <mergeCell ref="D153:D170"/>
+    <mergeCell ref="D171:D173"/>
   </mergeCells>
-  <conditionalFormatting sqref="G2:G155">
+  <conditionalFormatting sqref="G153:G173 G2:G152">
     <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
@@ -7873,11 +8362,11 @@
   </conditionalFormatting>
   <dataValidations count="4">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I55 I56:I105"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G152 G2:G55 G56:G106 G107:G123 G124:G135 G136:G151 G153:G155">
+    <dataValidation allowBlank="1" showErrorMessage="1" sqref="H152 H2:H55 H56:H106 H107:H123 H124:H135 H171:H173"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G152 G2:G55 G56:G106 G107:G123 G124:G135 G136:G151 G153:G170 G171:G173">
       <formula1>"Pass,Fail"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" sqref="H152 H2:H55 H56:H106 H107:H123 H124:H135 H153:H155"/>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" promptTitle="PLS Select 请选择" sqref="F152 F2:F55 F56:F106 F107:F123 F124:F135 F136:F151 F153:F155">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" promptTitle="PLS Select 请选择" sqref="F152 F153 F2:F55 F56:F106 F107:F123 F124:F135 F136:F151 F154:F170 F171:F173">
       <formula1>"是,否"</formula1>
     </dataValidation>
   </dataValidations>
@@ -7898,7 +8387,8 @@
     <hyperlink ref="D136" r:id="rId14" display="lvs-keepalived.md"/>
     <hyperlink ref="D136:D151" r:id="rId15" display="lvs-keepalived.md"/>
     <hyperlink ref="D152" r:id="rId16" display="kops.md"/>
-    <hyperlink ref="D153:D155" r:id="rId17" display="cadvisor.md"/>
+    <hyperlink ref="D171:D173" r:id="rId17" display="cadvisor.md"/>
+    <hyperlink ref="D153:D170" r:id="rId18" display="ovs.sh"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.510416666666667" footer="0.510416666666667"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>